<commit_message>
Actualización de dependencias y mejora de los componentes Abusos, Dashboard y Route-Creator
- React-router-dom se ha reducido a la versión 6.30.3 para compatibilidad.
- Se añadió la biblioteca xlsx para la exportación a Excel.
- Se ha implementado un mecanismo de notificación de actualizaciones entre los componentes AbusosTable y Stats.
- Componente Dashboard mejorado con nuevas funciones de filtrado y exportación de datos.
- Se ha mejorado la gestión y presentación de datos en Dashboard, incluyendo un formato numérico compacto.
- Se ha añadido un efecto de desplazamiento para los marcadores de caseta en el componente Route-Creator.
- Se ha refactorizado AbusosTable para notificar al componente principal sobre las actualizaciones.
- Se ha actualizado el componente Stats para reflejar los cambios en la estructura de datos y mejorar la lógica de renderizado.
- CrucesTable mejorado con una mejor gestión de las importaciones.
</commit_message>
<xml_diff>
--- a/Diagrama de Gantt IAVE.xlsx
+++ b/Diagrama de Gantt IAVE.xlsx
@@ -2838,9 +2838,6 @@
     <xf numFmtId="171" fontId="0" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="170" fontId="7" fillId="0" borderId="3" xfId="9">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="5" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2855,6 +2852,9 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="8" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="3" xfId="9">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="54">
@@ -10400,10 +10400,10 @@
   <dimension ref="A1:MW115"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="70" workbookViewId="0">
-      <pane xSplit="8" ySplit="7" topLeftCell="I87" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="8" ySplit="7" topLeftCell="I98" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="I1" sqref="I1"/>
       <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
-      <selection pane="bottomRight" activeCell="F91" sqref="F91:G91"/>
+      <selection pane="bottomRight" activeCell="D103" sqref="D103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -10449,10 +10449,10 @@
   <sheetData>
     <row r="1" spans="1:361" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A1"/>
-      <c r="B1" s="236" t="s">
+      <c r="B1" s="235" t="s">
         <v>31</v>
       </c>
-      <c r="C1" s="236"/>
+      <c r="C1" s="235"/>
       <c r="D1" s="1"/>
       <c r="E1" s="2"/>
       <c r="F1" s="4"/>
@@ -10466,38 +10466,38 @@
       <c r="A2" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="237" t="s">
+      <c r="B2" s="236" t="s">
         <v>32</v>
       </c>
-      <c r="C2" s="237"/>
+      <c r="C2" s="236"/>
       <c r="L2" s="39"/>
     </row>
     <row r="3" spans="1:361" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A3" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="238" t="s">
+      <c r="B3" s="237" t="s">
         <v>33</v>
       </c>
-      <c r="C3" s="238"/>
-      <c r="D3" s="239" t="s">
+      <c r="C3" s="237"/>
+      <c r="D3" s="238" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="240"/>
-      <c r="F3" s="235">
+      <c r="E3" s="239"/>
+      <c r="F3" s="240">
         <v>45714</v>
       </c>
-      <c r="G3" s="235"/>
+      <c r="G3" s="240"/>
     </row>
     <row r="4" spans="1:361" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="29" t="s">
         <v>2</v>
       </c>
       <c r="C4" s="53"/>
-      <c r="D4" s="239" t="s">
+      <c r="D4" s="238" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="240"/>
+      <c r="E4" s="239"/>
       <c r="F4" s="6">
         <v>49</v>
       </c>
@@ -45125,7 +45125,7 @@
         <v>271</v>
       </c>
       <c r="E91" s="214">
-        <v>0.1</v>
+        <v>0.8</v>
       </c>
       <c r="F91" s="215">
         <v>27</v>
@@ -49557,7 +49557,7 @@
         <v>264</v>
       </c>
       <c r="E103" s="214">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F103" s="226">
         <v>46051</v>
@@ -54372,50 +54372,6 @@
     </row>
   </sheetData>
   <mergeCells count="56">
-    <mergeCell ref="MC4:MI4"/>
-    <mergeCell ref="MJ4:MP4"/>
-    <mergeCell ref="MQ4:MW4"/>
-    <mergeCell ref="KT4:KZ4"/>
-    <mergeCell ref="LA4:LG4"/>
-    <mergeCell ref="LH4:LN4"/>
-    <mergeCell ref="LO4:LU4"/>
-    <mergeCell ref="LV4:MB4"/>
-    <mergeCell ref="JK4:JQ4"/>
-    <mergeCell ref="JR4:JX4"/>
-    <mergeCell ref="JY4:KE4"/>
-    <mergeCell ref="KF4:KL4"/>
-    <mergeCell ref="KM4:KS4"/>
-    <mergeCell ref="IB4:IH4"/>
-    <mergeCell ref="II4:IO4"/>
-    <mergeCell ref="IP4:IV4"/>
-    <mergeCell ref="IW4:JC4"/>
-    <mergeCell ref="JD4:JJ4"/>
-    <mergeCell ref="GS4:GY4"/>
-    <mergeCell ref="GZ4:HF4"/>
-    <mergeCell ref="HG4:HM4"/>
-    <mergeCell ref="HN4:HT4"/>
-    <mergeCell ref="HU4:IA4"/>
-    <mergeCell ref="FJ4:FP4"/>
-    <mergeCell ref="FQ4:FW4"/>
-    <mergeCell ref="FX4:GD4"/>
-    <mergeCell ref="GE4:GK4"/>
-    <mergeCell ref="GL4:GR4"/>
-    <mergeCell ref="EA4:EG4"/>
-    <mergeCell ref="EH4:EN4"/>
-    <mergeCell ref="EO4:EU4"/>
-    <mergeCell ref="EV4:FB4"/>
-    <mergeCell ref="FC4:FI4"/>
-    <mergeCell ref="DT4:DZ4"/>
-    <mergeCell ref="CK4:CQ4"/>
-    <mergeCell ref="CR4:CX4"/>
-    <mergeCell ref="CY4:DE4"/>
-    <mergeCell ref="DF4:DL4"/>
-    <mergeCell ref="DM4:DS4"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="D4:E4"/>
     <mergeCell ref="CD4:CJ4"/>
     <mergeCell ref="F3:G3"/>
     <mergeCell ref="L4:R4"/>
@@ -54428,6 +54384,50 @@
     <mergeCell ref="BI4:BO4"/>
     <mergeCell ref="BP4:BV4"/>
     <mergeCell ref="BW4:CC4"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="DT4:DZ4"/>
+    <mergeCell ref="CK4:CQ4"/>
+    <mergeCell ref="CR4:CX4"/>
+    <mergeCell ref="CY4:DE4"/>
+    <mergeCell ref="DF4:DL4"/>
+    <mergeCell ref="DM4:DS4"/>
+    <mergeCell ref="EA4:EG4"/>
+    <mergeCell ref="EH4:EN4"/>
+    <mergeCell ref="EO4:EU4"/>
+    <mergeCell ref="EV4:FB4"/>
+    <mergeCell ref="FC4:FI4"/>
+    <mergeCell ref="FJ4:FP4"/>
+    <mergeCell ref="FQ4:FW4"/>
+    <mergeCell ref="FX4:GD4"/>
+    <mergeCell ref="GE4:GK4"/>
+    <mergeCell ref="GL4:GR4"/>
+    <mergeCell ref="GS4:GY4"/>
+    <mergeCell ref="GZ4:HF4"/>
+    <mergeCell ref="HG4:HM4"/>
+    <mergeCell ref="HN4:HT4"/>
+    <mergeCell ref="HU4:IA4"/>
+    <mergeCell ref="IB4:IH4"/>
+    <mergeCell ref="II4:IO4"/>
+    <mergeCell ref="IP4:IV4"/>
+    <mergeCell ref="IW4:JC4"/>
+    <mergeCell ref="JD4:JJ4"/>
+    <mergeCell ref="JK4:JQ4"/>
+    <mergeCell ref="JR4:JX4"/>
+    <mergeCell ref="JY4:KE4"/>
+    <mergeCell ref="KF4:KL4"/>
+    <mergeCell ref="KM4:KS4"/>
+    <mergeCell ref="MC4:MI4"/>
+    <mergeCell ref="MJ4:MP4"/>
+    <mergeCell ref="MQ4:MW4"/>
+    <mergeCell ref="KT4:KZ4"/>
+    <mergeCell ref="LA4:LG4"/>
+    <mergeCell ref="LH4:LN4"/>
+    <mergeCell ref="LO4:LU4"/>
+    <mergeCell ref="LV4:MB4"/>
   </mergeCells>
   <conditionalFormatting sqref="E114:E115 E24:E28 E31:E33 E7:E22 E38 E36 E41:E43 E61:E86 E47:E58">
     <cfRule type="dataBar" priority="982">
@@ -58285,6 +58285,35 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Url xsi:nil="true"/>
+      <Description xsi:nil="true"/>
+    </Image>
+    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
+    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </ImageTagsTaxHTField>
+    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
+    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010079F111ED35F8CC479449609E8A0923A6" ma:contentTypeVersion="24" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="2d714a3296df14eba7a100bb665443ca">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xmlns:ns3="16c05727-aa75-4e4a-9b5f-8a80a1165891" xmlns:ns4="230e9df3-be65-4c73-a93b-d1236ebd677e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="49549bf45bfbbfb6cffed527380e77e1" ns1:_="" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -58572,36 +58601,34 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5144944C-1F1D-4162-962A-96F3FC8455D8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="16c05727-aa75-4e4a-9b5f-8a80a1165891"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Url xsi:nil="true"/>
-      <Description xsi:nil="true"/>
-    </Image>
-    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
-    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </ImageTagsTaxHTField>
-    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
-    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8FE8ED85-58B3-4608-8E91-0433556D50CE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{708DBB9E-6D89-4A94-9DC5-964B7833E11C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -58620,31 +58647,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8FE8ED85-58B3-4608-8E91-0433556D50CE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5144944C-1F1D-4162-962A-96F3FC8455D8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="16c05727-aa75-4e4a-9b5f-8a80a1165891"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
-    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>